<commit_message>
Se modifican lista de niveles. Códigos 07 y 08. Se elimina la coma
</commit_message>
<xml_diff>
--- a/ede/ede/listValidationData.xlsx
+++ b/ede/ede/listValidationData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dockerETL\DockerCode\DockerEdeCode\ede\ede\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD353BEF-8CC9-4DCF-9C87-44E907340B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC44405-2A9E-4A85-BA22-9CE322B20311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ListValidations" sheetId="1" r:id="rId1"/>
@@ -196,9 +196,6 @@
     <t>Quechua</t>
   </si>
   <si>
-    <t>07:Enseñanza Media Técnico Profesional y Artística, Jóvenes</t>
-  </si>
-  <si>
     <t>800:Marítima</t>
   </si>
   <si>
@@ -217,9 +214,6 @@
     <t>Rapa-Nui o Pascuense</t>
   </si>
   <si>
-    <t>08:Educación Media Técnico Profesional y Artística, Adultos</t>
-  </si>
-  <si>
     <t>900:Artística</t>
   </si>
   <si>
@@ -1094,6 +1088,12 @@
   </si>
   <si>
     <t>03:AulaHospitalaria</t>
+  </si>
+  <si>
+    <t>07:Enseñanza Media Técnico Profesional y Artística (Jóvenes)</t>
+  </si>
+  <si>
+    <t>08:Educación Media Técnico Profesional y Artística (Adultos)</t>
   </si>
 </sst>
 </file>
@@ -1349,14 +1349,14 @@
   </sheetPr>
   <dimension ref="A1:J2013"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="55.6640625" bestFit="1" customWidth="1"/>
@@ -1492,7 +1492,7 @@
         <v>34</v>
       </c>
       <c r="J4" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1572,1257 +1572,1257 @@
         <v>57</v>
       </c>
       <c r="B8" t="s">
+        <v>356</v>
+      </c>
+      <c r="C8" t="s">
         <v>58</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>59</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>60</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>61</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>62</v>
-      </c>
-      <c r="G8" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" t="s">
+        <v>357</v>
+      </c>
+      <c r="C9" t="s">
         <v>64</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>65</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>66</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>67</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>68</v>
-      </c>
-      <c r="F9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" t="s">
         <v>71</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>72</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>73</v>
-      </c>
-      <c r="F10" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" t="s">
         <v>76</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>77</v>
-      </c>
-      <c r="F11" t="s">
-        <v>78</v>
-      </c>
-      <c r="G11" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" t="s">
         <v>80</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
         <v>81</v>
-      </c>
-      <c r="F12" t="s">
-        <v>82</v>
-      </c>
-      <c r="G12" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" t="s">
         <v>84</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>85</v>
-      </c>
-      <c r="F13" t="s">
-        <v>86</v>
-      </c>
-      <c r="G13" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" t="s">
         <v>88</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>89</v>
-      </c>
-      <c r="F14" t="s">
-        <v>90</v>
-      </c>
-      <c r="G14" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" t="s">
         <v>92</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>93</v>
-      </c>
-      <c r="F15" t="s">
-        <v>94</v>
-      </c>
-      <c r="G15" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" t="s">
         <v>96</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>97</v>
-      </c>
-      <c r="F16" t="s">
-        <v>98</v>
-      </c>
-      <c r="G16" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="17" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" t="s">
         <v>100</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
         <v>101</v>
-      </c>
-      <c r="F17" t="s">
-        <v>102</v>
-      </c>
-      <c r="G17" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="18" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" t="s">
         <v>104</v>
       </c>
-      <c r="E18" t="s">
+      <c r="G18" t="s">
         <v>105</v>
-      </c>
-      <c r="F18" t="s">
-        <v>106</v>
-      </c>
-      <c r="G18" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="19" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" t="s">
         <v>108</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>109</v>
-      </c>
-      <c r="F19" t="s">
-        <v>110</v>
-      </c>
-      <c r="G19" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="20" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20" t="s">
         <v>112</v>
       </c>
-      <c r="E20" t="s">
+      <c r="G20" t="s">
         <v>113</v>
-      </c>
-      <c r="F20" t="s">
-        <v>114</v>
-      </c>
-      <c r="G20" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="21" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" t="s">
         <v>116</v>
       </c>
-      <c r="E21" t="s">
+      <c r="G21" t="s">
         <v>117</v>
-      </c>
-      <c r="F21" t="s">
-        <v>118</v>
-      </c>
-      <c r="G21" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="22" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
+        <v>118</v>
+      </c>
+      <c r="E22" t="s">
+        <v>119</v>
+      </c>
+      <c r="F22" t="s">
         <v>120</v>
       </c>
-      <c r="E22" t="s">
+      <c r="G22" t="s">
         <v>121</v>
-      </c>
-      <c r="F22" t="s">
-        <v>122</v>
-      </c>
-      <c r="G22" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="23" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
+        <v>122</v>
+      </c>
+      <c r="F23" t="s">
+        <v>123</v>
+      </c>
+      <c r="G23" t="s">
         <v>124</v>
-      </c>
-      <c r="F23" t="s">
-        <v>125</v>
-      </c>
-      <c r="G23" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="24" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
+        <v>125</v>
+      </c>
+      <c r="F24" t="s">
+        <v>126</v>
+      </c>
+      <c r="G24" t="s">
         <v>127</v>
-      </c>
-      <c r="F24" t="s">
-        <v>128</v>
-      </c>
-      <c r="G24" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="25" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
+        <v>128</v>
+      </c>
+      <c r="F25" t="s">
+        <v>129</v>
+      </c>
+      <c r="G25" t="s">
         <v>130</v>
-      </c>
-      <c r="F25" t="s">
-        <v>131</v>
-      </c>
-      <c r="G25" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="26" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
+        <v>131</v>
+      </c>
+      <c r="F26" t="s">
+        <v>132</v>
+      </c>
+      <c r="G26" t="s">
         <v>133</v>
-      </c>
-      <c r="F26" t="s">
-        <v>134</v>
-      </c>
-      <c r="G26" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="27" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
+        <v>134</v>
+      </c>
+      <c r="F27" t="s">
+        <v>135</v>
+      </c>
+      <c r="G27" t="s">
         <v>136</v>
-      </c>
-      <c r="F27" t="s">
-        <v>137</v>
-      </c>
-      <c r="G27" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="28" spans="4:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
+        <v>137</v>
+      </c>
+      <c r="F28" t="s">
+        <v>138</v>
+      </c>
+      <c r="G28" t="s">
         <v>139</v>
-      </c>
-      <c r="F28" t="s">
-        <v>140</v>
-      </c>
-      <c r="G28" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="29" spans="4:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
+        <v>140</v>
+      </c>
+      <c r="F29" t="s">
+        <v>141</v>
+      </c>
+      <c r="G29" t="s">
         <v>142</v>
-      </c>
-      <c r="F29" t="s">
-        <v>143</v>
-      </c>
-      <c r="G29" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="30" spans="4:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
+        <v>143</v>
+      </c>
+      <c r="F30" t="s">
+        <v>144</v>
+      </c>
+      <c r="G30" t="s">
         <v>145</v>
-      </c>
-      <c r="F30" t="s">
-        <v>146</v>
-      </c>
-      <c r="G30" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="31" spans="4:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
+        <v>146</v>
+      </c>
+      <c r="F31" t="s">
+        <v>147</v>
+      </c>
+      <c r="G31" t="s">
         <v>148</v>
-      </c>
-      <c r="F31" t="s">
-        <v>149</v>
-      </c>
-      <c r="G31" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="32" spans="4:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
+        <v>149</v>
+      </c>
+      <c r="F32" t="s">
+        <v>150</v>
+      </c>
+      <c r="G32" t="s">
         <v>151</v>
-      </c>
-      <c r="F32" t="s">
-        <v>152</v>
-      </c>
-      <c r="G32" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="33" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
+        <v>152</v>
+      </c>
+      <c r="F33" t="s">
+        <v>153</v>
+      </c>
+      <c r="G33" t="s">
         <v>154</v>
-      </c>
-      <c r="F33" t="s">
-        <v>155</v>
-      </c>
-      <c r="G33" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="34" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
+        <v>155</v>
+      </c>
+      <c r="F34" t="s">
+        <v>156</v>
+      </c>
+      <c r="G34" t="s">
         <v>157</v>
-      </c>
-      <c r="F34" t="s">
-        <v>158</v>
-      </c>
-      <c r="G34" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="35" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
+        <v>158</v>
+      </c>
+      <c r="F35" t="s">
+        <v>159</v>
+      </c>
+      <c r="G35" t="s">
         <v>160</v>
-      </c>
-      <c r="F35" t="s">
-        <v>161</v>
-      </c>
-      <c r="G35" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="36" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
+        <v>161</v>
+      </c>
+      <c r="F36" t="s">
+        <v>162</v>
+      </c>
+      <c r="G36" t="s">
         <v>163</v>
-      </c>
-      <c r="F36" t="s">
-        <v>164</v>
-      </c>
-      <c r="G36" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="37" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
+        <v>164</v>
+      </c>
+      <c r="F37" t="s">
+        <v>165</v>
+      </c>
+      <c r="G37" t="s">
         <v>166</v>
-      </c>
-      <c r="F37" t="s">
-        <v>167</v>
-      </c>
-      <c r="G37" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="38" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
+        <v>167</v>
+      </c>
+      <c r="F38" t="s">
+        <v>168</v>
+      </c>
+      <c r="G38" t="s">
         <v>169</v>
-      </c>
-      <c r="F38" t="s">
-        <v>170</v>
-      </c>
-      <c r="G38" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="39" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
+        <v>170</v>
+      </c>
+      <c r="F39" t="s">
+        <v>171</v>
+      </c>
+      <c r="G39" t="s">
         <v>172</v>
-      </c>
-      <c r="F39" t="s">
-        <v>173</v>
-      </c>
-      <c r="G39" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="40" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
+        <v>173</v>
+      </c>
+      <c r="F40" t="s">
+        <v>174</v>
+      </c>
+      <c r="G40" t="s">
         <v>175</v>
-      </c>
-      <c r="F40" t="s">
-        <v>176</v>
-      </c>
-      <c r="G40" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="41" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
+        <v>176</v>
+      </c>
+      <c r="F41" t="s">
+        <v>177</v>
+      </c>
+      <c r="G41" t="s">
         <v>178</v>
-      </c>
-      <c r="F41" t="s">
-        <v>179</v>
-      </c>
-      <c r="G41" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="42" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
+        <v>179</v>
+      </c>
+      <c r="F42" t="s">
+        <v>180</v>
+      </c>
+      <c r="G42" t="s">
         <v>181</v>
-      </c>
-      <c r="F42" t="s">
-        <v>182</v>
-      </c>
-      <c r="G42" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="43" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G43" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="44" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G44" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="45" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G45" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G46" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="47" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G47" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="48" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E48" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G48" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="49" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G49" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="50" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E50" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G50" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="51" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E51" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G51" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="52" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G52" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="53" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G53" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="54" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E54" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G54" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E55" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G55" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="56" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G56" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="57" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G57" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="58" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E58" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G58" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="59" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E59" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G59" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="60" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G60" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="61" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E61" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G61" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="62" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E62" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G62" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="63" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G63" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="64" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E64" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G64" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="65" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E65" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G65" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="66" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E66" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G66" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="67" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E67" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G67" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="68" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E68" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G68" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="69" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E69" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G69" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="70" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E70" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G70" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="71" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E71" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G71" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="72" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G72" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="73" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G73" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="74" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G74" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="75" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G75" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="76" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G76" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="77" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G77" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="78" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G78" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="79" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G79" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="80" spans="5:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G80" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="81" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G81" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="82" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G82" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="83" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G83" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="84" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G84" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="85" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G85" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="86" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G86" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="87" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G87" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="88" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G88" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="89" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G89" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="90" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G90" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="91" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G91" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="92" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G92" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="93" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G93" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="94" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G94" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="95" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G95" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="96" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G96" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="97" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G97" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="98" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G98" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="99" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G99" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="100" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G100" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="101" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G101" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="102" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G102" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="103" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G103" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="104" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G104" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="105" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G105" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="106" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G106" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="107" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G107" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="108" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G108" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="109" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G109" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="110" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G110" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="111" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G111" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="112" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G112" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="113" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G113" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="114" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G114" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="115" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G115" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="116" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G116" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="117" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G117" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="118" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G118" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="119" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G119" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="120" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G120" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="121" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G121" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="122" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G122" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="123" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G123" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="124" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G124" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="125" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G125" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="126" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G126" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="127" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G127" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="128" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G128" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="129" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G129" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="130" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G130" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="131" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G131" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="132" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G132" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="133" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G133" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="134" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G134" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="135" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G135" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="136" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G136" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="137" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G137" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="138" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G138" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="139" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G139" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="140" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G140" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="141" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G141" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="142" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G142" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="143" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G143" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="144" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G144" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="145" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G145" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="146" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G146" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="147" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G147" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="148" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G148" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="149" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G149" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="150" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G150" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="151" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G151" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="152" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G152" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="153" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G153" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="154" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G154" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="155" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G155" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="156" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G156" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="157" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G157" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="158" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G158" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="159" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G159" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="160" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G160" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="161" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G161" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="162" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G162" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="163" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G163" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="164" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G164" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="165" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G165" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="166" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G166" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="167" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G167" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="168" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G168" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="169" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G169" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="170" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G170" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="171" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G171" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="172" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G172" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="173" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G173" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="174" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G174" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="175" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G175" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="176" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G176" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="177" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G177" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="178" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G178" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="179" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G179" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="180" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G180" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="181" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G181" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="182" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G182" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="183" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G183" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="184" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G184" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="185" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G185" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="186" spans="7:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G186" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="187" spans="7:7" ht="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
se agregan columnas numeroREX y fechaREX en tabla organizationCalendarSession para identificar REX que autoriza reemplazo
</commit_message>
<xml_diff>
--- a/ede/ede/listValidationData.xlsx
+++ b/ede/ede/listValidationData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dockerETL\DockerCode\DockerEdeCode\ede\ede\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC44405-2A9E-4A85-BA22-9CE322B20311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8207B0C2-AFF8-4029-9719-D0C390E8B655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ListValidations" sheetId="1" r:id="rId1"/>
@@ -1350,7 +1350,7 @@
   <dimension ref="A1:J2013"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>